<commit_message>
Make figure 27 (land cover change) tables for Jessica at county and regional level
</commit_message>
<xml_diff>
--- a/Tables/Fig35_Table_Projected_LU.xlsx
+++ b/Tables/Fig35_Table_Projected_LU.xlsx
@@ -96,28 +96,36 @@
     <t>Baltimore City</t>
   </si>
   <si>
-    <t>Impervious Roads</t>
-  </si>
-  <si>
-    <t>Impervious Non-Roads</t>
-  </si>
-  <si>
-    <t>Tree Canopy Over Impervious</t>
+    <t>Impervious
+Roads</t>
+  </si>
+  <si>
+    <t>Impervious
+Non-Roads</t>
+  </si>
+  <si>
+    <t>Tree Canopy
+Over
+Impervious</t>
   </si>
   <si>
     <t>Turf Grass</t>
   </si>
   <si>
-    <t>Tree Canopy over Turf Grass</t>
+    <t>Tree Canopy
+over Turf
+Grass</t>
   </si>
   <si>
     <t>Forest</t>
   </si>
   <si>
-    <t>Wetlands (Other)</t>
-  </si>
-  <si>
-    <t>Wetlands (Floodplain)</t>
+    <t>Wetlands
+(Other)</t>
+  </si>
+  <si>
+    <t>Wetlands
+(Floodplain)</t>
   </si>
   <si>
     <t>Mixed Open</t>
@@ -3208,10 +3216,10 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C8" t="n">
-        <v>1498.9165000000096</v>
+        <v>4378.526799999998</v>
       </c>
     </row>
     <row r="9">
@@ -3219,10 +3227,10 @@
         <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="n">
-        <v>4378.526799999998</v>
+        <v>1498.9165000000096</v>
       </c>
     </row>
     <row r="10">
@@ -3329,10 +3337,10 @@
         <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" t="n">
-        <v>60.439300000001026</v>
+        <v>405.1715999999999</v>
       </c>
     </row>
     <row r="20">
@@ -3340,10 +3348,10 @@
         <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" t="n">
-        <v>405.1715999999999</v>
+        <v>60.439300000001026</v>
       </c>
     </row>
     <row r="21">
@@ -3450,10 +3458,10 @@
         <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C30" t="n">
-        <v>563.6491999999998</v>
+        <v>1920.5349000000042</v>
       </c>
     </row>
     <row r="31">
@@ -3461,10 +3469,10 @@
         <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" t="n">
-        <v>1920.5349000000042</v>
+        <v>563.6491999999998</v>
       </c>
     </row>
     <row r="32">
@@ -3571,10 +3579,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C41" t="n">
-        <v>414.71030000000997</v>
+        <v>3379.5023999999903</v>
       </c>
     </row>
     <row r="42">
@@ -3582,10 +3590,10 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C42" t="n">
-        <v>3379.5023999999903</v>
+        <v>414.71030000000997</v>
       </c>
     </row>
     <row r="43">
@@ -3692,10 +3700,10 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C52" t="n">
-        <v>211.66100000000102</v>
+        <v>1213.99970000002</v>
       </c>
     </row>
     <row r="53">
@@ -3703,10 +3711,10 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C53" t="n">
-        <v>1213.99970000002</v>
+        <v>211.66100000000102</v>
       </c>
     </row>
     <row r="54">
@@ -3813,10 +3821,10 @@
         <v>44</v>
       </c>
       <c r="B63" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C63" t="n">
-        <v>200.54460000001006</v>
+        <v>779.6855999999907</v>
       </c>
     </row>
     <row r="64">
@@ -3824,10 +3832,10 @@
         <v>44</v>
       </c>
       <c r="B64" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C64" t="n">
-        <v>779.6855999999907</v>
+        <v>200.54460000001006</v>
       </c>
     </row>
     <row r="65">

</xml_diff>